<commit_message>
Fix E7: define Gc in legacy edge evolution
- Replace undefined 'Gc' variable with 'fracture_Gc' parameter in
  _evolve_edges_legacy energy gate calculation (line 345)
- Remove skip markers from 4 E7 tests

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Fibrinet_APP/tests/input_data/Hangman.xlsx
+++ b/Fibrinet_APP/tests/input_data/Hangman.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Documents\GitHub\Webslinger\test\input_data\INPUT TESTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manda\Documents\UCO\Fibrinet-main\Fibrinet_APP\test\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4359368-B45F-4F94-938C-9572280BD922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911BF8CC-82C8-4ECA-A5B5-CA4F2F4C2B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>n_id</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>spring_stiffness_constant</t>
+  </si>
+  <si>
+    <t>thickness</t>
+  </si>
+  <si>
+    <t>is_left_boundary</t>
+  </si>
+  <si>
+    <t>is_right_boundary</t>
   </si>
 </sst>
 </file>
@@ -101,25 +110,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,230 +430,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="E1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
         <v>2</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>8</v>
       </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>4</v>
       </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>7</v>
       </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>8</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>8</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>8</v>
       </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>1</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>124.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>2</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="5">
         <v>2</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="5">
         <v>4</v>
       </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>194.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>3</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="5">
         <v>4</v>
       </c>
-      <c r="D12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>167.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
         <v>4</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="5">
         <v>3</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>5</v>
       </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>151.80000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>5</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="5">
         <v>4</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="5">
         <v>6</v>
       </c>
-      <c r="D14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>98.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>